<commit_message>
added  BugReport.xlsx second attempt
</commit_message>
<xml_diff>
--- a/bug_report/BugReport.xlsx
+++ b/bug_report/BugReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MacBook Air\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MacBook Air\Desktop\gitTest2\SecondRepository\bug_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0F03F3-8371-458C-8B90-2E7F0C19C436}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BF5A68-BB63-4E20-8DB7-6A434CDF0B85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9075" xr2:uid="{C399A4AF-B58C-4B71-8E99-079B9BC3C45E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Summary</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>1BR</t>
   </si>
 </sst>
 </file>
@@ -170,23 +173,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -194,26 +212,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,7 +535,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,160 +546,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="12" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:F4"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
@@ -707,12 +716,6 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C12"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:F4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>